<commit_message>
update users roles 1
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/828d708a985a52d0/Bureau/AffiKoue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{B8176D72-3CC7-467C-A60C-A52FCC3E6683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38596EE9-ACAB-46B0-B3AA-ECD1C5B9391F}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{B8176D72-3CC7-467C-A60C-A52FCC3E6683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0411FA5-7295-414A-812E-DBE4B4DD6071}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49A121DB-F08D-4D32-A08B-A0BD9ADB553E}"/>
   </bookViews>
@@ -492,19 +492,20 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>